<commit_message>
changed : complete __meta_schema__ variable and remove virtual table
</commit_message>
<xml_diff>
--- a/public/data/db_source/__meta_schema__.xlsx
+++ b/public/data/db_source/__meta_schema__.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bassim/code/datannur/datannur_dev/public/data/db_source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{689C9828-6427-FA48-8433-DACF502CA567}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4638EFDA-B734-1943-A292-852528CDDEDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2680" yWindow="500" windowWidth="26120" windowHeight="17500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="513" uniqueCount="189">
   <si>
     <t>id</t>
   </si>
@@ -561,16 +561,64 @@
   </si>
   <si>
     <t>Variables contenues dans les datasets</t>
+  </si>
+  <si>
+    <t>tag_ids</t>
+  </si>
+  <si>
+    <t>doc_ids</t>
+  </si>
+  <si>
+    <t>last_update</t>
+  </si>
+  <si>
+    <t>timestamp unix de la dernière modification</t>
+  </si>
+  <si>
+    <t>clés des docs liés</t>
+  </si>
+  <si>
+    <t>clés des mots clés liés</t>
+  </si>
+  <si>
+    <t>clé du mot clé parent</t>
+  </si>
+  <si>
+    <t>original_name</t>
+  </si>
+  <si>
+    <t>modality_ids</t>
+  </si>
+  <si>
+    <t>nom d'origine de la variable</t>
+  </si>
+  <si>
+    <t>début de la période couverte par la variable</t>
+  </si>
+  <si>
+    <t>fin de la période couverte par la variable</t>
+  </si>
+  <si>
+    <t>clé des modalités liées</t>
+  </si>
+  <si>
+    <t>timestamp unix de l'ajout du favori</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -596,8 +644,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -616,10 +665,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{CC52189E-6718-7640-A09D-3E13A3AE1ED2}" name="Tableau3" displayName="Tableau3" ref="A1:D120" totalsRowShown="0">
-  <autoFilter ref="A1:D120" xr:uid="{CC52189E-6718-7640-A09D-3E13A3AE1ED2}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D120">
-    <sortCondition ref="A1:A120"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{CC52189E-6718-7640-A09D-3E13A3AE1ED2}" name="Tableau3" displayName="Tableau3" ref="A1:D134" totalsRowShown="0">
+  <autoFilter ref="A1:D134" xr:uid="{CC52189E-6718-7640-A09D-3E13A3AE1ED2}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D134">
+    <sortCondition ref="A1:A134"/>
   </sortState>
   <tableColumns count="4">
     <tableColumn id="4" xr3:uid="{D4AE5F0B-EFF7-F144-B9F0-6F582D88D1B3}" name="folder"/>
@@ -953,11 +1002,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D120"/>
+  <dimension ref="A1:D134"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" showRuler="0" zoomScale="125" zoomScaleNormal="140" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A106" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D119" sqref="D119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1336,10 +1385,13 @@
         <v>152</v>
       </c>
       <c r="B28" t="s">
-        <v>110</v>
+        <v>8</v>
+      </c>
+      <c r="C28" t="s">
+        <v>175</v>
       </c>
       <c r="D28" t="s">
-        <v>159</v>
+        <v>180</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
@@ -1347,13 +1399,13 @@
         <v>152</v>
       </c>
       <c r="B29" t="s">
-        <v>110</v>
+        <v>8</v>
       </c>
       <c r="C29" t="s">
-        <v>2</v>
+        <v>176</v>
       </c>
       <c r="D29" t="s">
-        <v>66</v>
+        <v>179</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
@@ -1363,11 +1415,8 @@
       <c r="B30" t="s">
         <v>110</v>
       </c>
-      <c r="C30" t="s">
-        <v>83</v>
-      </c>
       <c r="D30" t="s">
-        <v>126</v>
+        <v>159</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
@@ -1378,10 +1427,10 @@
         <v>110</v>
       </c>
       <c r="C31" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D31" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
@@ -1392,10 +1441,10 @@
         <v>110</v>
       </c>
       <c r="C32" t="s">
-        <v>0</v>
+        <v>83</v>
       </c>
       <c r="D32" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
@@ -1406,10 +1455,10 @@
         <v>110</v>
       </c>
       <c r="C33" t="s">
-        <v>96</v>
+        <v>9</v>
       </c>
       <c r="D33" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
@@ -1420,10 +1469,10 @@
         <v>110</v>
       </c>
       <c r="C34" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D34" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
@@ -1434,10 +1483,10 @@
         <v>110</v>
       </c>
       <c r="C35" t="s">
-        <v>111</v>
+        <v>96</v>
       </c>
       <c r="D35" t="s">
-        <v>129</v>
+        <v>67</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
@@ -1448,10 +1497,10 @@
         <v>110</v>
       </c>
       <c r="C36" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D36" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
@@ -1459,10 +1508,13 @@
         <v>152</v>
       </c>
       <c r="B37" t="s">
-        <v>112</v>
+        <v>110</v>
+      </c>
+      <c r="C37" t="s">
+        <v>111</v>
       </c>
       <c r="D37" t="s">
-        <v>161</v>
+        <v>129</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
@@ -1470,13 +1522,13 @@
         <v>152</v>
       </c>
       <c r="B38" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C38" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D38" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
@@ -1484,13 +1536,13 @@
         <v>152</v>
       </c>
       <c r="B39" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C39" t="s">
-        <v>4</v>
+        <v>177</v>
       </c>
       <c r="D39" t="s">
-        <v>131</v>
+        <v>178</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
@@ -1498,10 +1550,10 @@
         <v>152</v>
       </c>
       <c r="B40" t="s">
-        <v>26</v>
+        <v>112</v>
       </c>
       <c r="D40" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
@@ -1509,13 +1561,13 @@
         <v>152</v>
       </c>
       <c r="B41" t="s">
-        <v>26</v>
+        <v>112</v>
       </c>
       <c r="C41" t="s">
-        <v>142</v>
+        <v>0</v>
       </c>
       <c r="D41" t="s">
-        <v>149</v>
+        <v>130</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
@@ -1523,13 +1575,13 @@
         <v>152</v>
       </c>
       <c r="B42" t="s">
-        <v>26</v>
+        <v>112</v>
       </c>
       <c r="C42" t="s">
-        <v>102</v>
+        <v>4</v>
       </c>
       <c r="D42" t="s">
-        <v>103</v>
+        <v>131</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
@@ -1539,11 +1591,8 @@
       <c r="B43" t="s">
         <v>26</v>
       </c>
-      <c r="C43" t="s">
-        <v>1</v>
-      </c>
       <c r="D43" t="s">
-        <v>47</v>
+        <v>163</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
@@ -1554,10 +1603,10 @@
         <v>26</v>
       </c>
       <c r="C44" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="D44" t="s">
-        <v>139</v>
+        <v>149</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
@@ -1568,10 +1617,10 @@
         <v>26</v>
       </c>
       <c r="C45" t="s">
-        <v>145</v>
+        <v>102</v>
       </c>
       <c r="D45" t="s">
-        <v>146</v>
+        <v>103</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
@@ -1582,10 +1631,10 @@
         <v>26</v>
       </c>
       <c r="C46" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D46" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
@@ -1596,10 +1645,10 @@
         <v>26</v>
       </c>
       <c r="C47" t="s">
-        <v>15</v>
+        <v>136</v>
       </c>
       <c r="D47" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
@@ -1610,10 +1659,10 @@
         <v>26</v>
       </c>
       <c r="C48" t="s">
-        <v>109</v>
+        <v>145</v>
       </c>
       <c r="D48" t="s">
-        <v>137</v>
+        <v>146</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
@@ -1624,10 +1673,10 @@
         <v>26</v>
       </c>
       <c r="C49" t="s">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="D49" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
@@ -1638,10 +1687,10 @@
         <v>26</v>
       </c>
       <c r="C50" t="s">
-        <v>144</v>
+        <v>15</v>
       </c>
       <c r="D50" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
@@ -1652,10 +1701,10 @@
         <v>26</v>
       </c>
       <c r="C51" t="s">
-        <v>4</v>
+        <v>109</v>
       </c>
       <c r="D51" t="s">
-        <v>46</v>
+        <v>137</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
@@ -1666,10 +1715,10 @@
         <v>26</v>
       </c>
       <c r="C52" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D52" t="s">
-        <v>106</v>
+        <v>69</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
@@ -1680,10 +1729,10 @@
         <v>26</v>
       </c>
       <c r="C53" t="s">
-        <v>3</v>
+        <v>144</v>
       </c>
       <c r="D53" t="s">
-        <v>68</v>
+        <v>150</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
@@ -1694,10 +1743,10 @@
         <v>26</v>
       </c>
       <c r="C54" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="D54" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
@@ -1708,10 +1757,10 @@
         <v>26</v>
       </c>
       <c r="C55" t="s">
-        <v>135</v>
+        <v>10</v>
       </c>
       <c r="D55" t="s">
-        <v>138</v>
+        <v>106</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
@@ -1722,10 +1771,10 @@
         <v>26</v>
       </c>
       <c r="C56" t="s">
-        <v>101</v>
+        <v>3</v>
       </c>
       <c r="D56" t="s">
-        <v>104</v>
+        <v>68</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
@@ -1736,10 +1785,10 @@
         <v>26</v>
       </c>
       <c r="C57" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D57" t="s">
-        <v>147</v>
+        <v>48</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
@@ -1747,10 +1796,13 @@
         <v>152</v>
       </c>
       <c r="B58" t="s">
-        <v>113</v>
+        <v>26</v>
+      </c>
+      <c r="C58" t="s">
+        <v>135</v>
       </c>
       <c r="D58" t="s">
-        <v>164</v>
+        <v>138</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
@@ -1758,13 +1810,13 @@
         <v>152</v>
       </c>
       <c r="B59" t="s">
-        <v>113</v>
+        <v>26</v>
       </c>
       <c r="C59" t="s">
-        <v>0</v>
+        <v>101</v>
       </c>
       <c r="D59" t="s">
-        <v>133</v>
+        <v>104</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
@@ -1772,13 +1824,13 @@
         <v>152</v>
       </c>
       <c r="B60" t="s">
-        <v>113</v>
+        <v>26</v>
       </c>
       <c r="C60" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D60" t="s">
-        <v>134</v>
+        <v>147</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
@@ -1786,10 +1838,13 @@
         <v>152</v>
       </c>
       <c r="B61" t="s">
-        <v>95</v>
+        <v>26</v>
+      </c>
+      <c r="C61" t="s">
+        <v>175</v>
       </c>
       <c r="D61" t="s">
-        <v>165</v>
+        <v>180</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
@@ -1797,13 +1852,13 @@
         <v>152</v>
       </c>
       <c r="B62" t="s">
-        <v>95</v>
+        <v>26</v>
       </c>
       <c r="C62" t="s">
-        <v>1</v>
+        <v>176</v>
       </c>
       <c r="D62" t="s">
-        <v>6</v>
+        <v>179</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
@@ -1811,13 +1866,10 @@
         <v>152</v>
       </c>
       <c r="B63" t="s">
-        <v>95</v>
-      </c>
-      <c r="C63" t="s">
-        <v>97</v>
+        <v>113</v>
       </c>
       <c r="D63" t="s">
-        <v>99</v>
+        <v>164</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
@@ -1825,13 +1877,13 @@
         <v>152</v>
       </c>
       <c r="B64" t="s">
-        <v>95</v>
+        <v>113</v>
       </c>
       <c r="C64" t="s">
         <v>0</v>
       </c>
       <c r="D64" t="s">
-        <v>54</v>
+        <v>133</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
@@ -1839,13 +1891,13 @@
         <v>152</v>
       </c>
       <c r="B65" t="s">
-        <v>95</v>
+        <v>113</v>
       </c>
       <c r="C65" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="D65" t="s">
-        <v>5</v>
+        <v>134</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
@@ -1855,11 +1907,8 @@
       <c r="B66" t="s">
         <v>95</v>
       </c>
-      <c r="C66" t="s">
-        <v>3</v>
-      </c>
       <c r="D66" t="s">
-        <v>70</v>
+        <v>165</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
@@ -1870,10 +1919,10 @@
         <v>95</v>
       </c>
       <c r="C67" t="s">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="D67" t="s">
-        <v>49</v>
+        <v>6</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
@@ -1884,10 +1933,10 @@
         <v>95</v>
       </c>
       <c r="C68" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D68" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
@@ -1895,10 +1944,13 @@
         <v>152</v>
       </c>
       <c r="B69" t="s">
-        <v>28</v>
+        <v>95</v>
+      </c>
+      <c r="C69" t="s">
+        <v>0</v>
       </c>
       <c r="D69" t="s">
-        <v>167</v>
+        <v>54</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
@@ -1906,13 +1958,13 @@
         <v>152</v>
       </c>
       <c r="B70" t="s">
-        <v>28</v>
+        <v>95</v>
       </c>
       <c r="C70" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D70" t="s">
-        <v>61</v>
+        <v>5</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
@@ -1920,13 +1972,13 @@
         <v>152</v>
       </c>
       <c r="B71" t="s">
-        <v>28</v>
+        <v>95</v>
       </c>
       <c r="C71" t="s">
-        <v>96</v>
+        <v>3</v>
       </c>
       <c r="D71" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
@@ -1934,10 +1986,13 @@
         <v>152</v>
       </c>
       <c r="B72" t="s">
-        <v>71</v>
+        <v>95</v>
+      </c>
+      <c r="C72" t="s">
+        <v>14</v>
       </c>
       <c r="D72" t="s">
-        <v>168</v>
+        <v>49</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
@@ -1945,13 +2000,13 @@
         <v>152</v>
       </c>
       <c r="B73" t="s">
-        <v>71</v>
+        <v>95</v>
       </c>
       <c r="C73" t="s">
-        <v>1</v>
+        <v>98</v>
       </c>
       <c r="D73" t="s">
-        <v>72</v>
+        <v>100</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
@@ -1959,13 +2014,13 @@
         <v>152</v>
       </c>
       <c r="B74" t="s">
-        <v>71</v>
+        <v>95</v>
       </c>
       <c r="C74" t="s">
-        <v>9</v>
+        <v>175</v>
       </c>
       <c r="D74" t="s">
-        <v>114</v>
+        <v>180</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
@@ -1973,13 +2028,13 @@
         <v>152</v>
       </c>
       <c r="B75" t="s">
-        <v>71</v>
+        <v>95</v>
       </c>
       <c r="C75" t="s">
-        <v>0</v>
+        <v>176</v>
       </c>
       <c r="D75" t="s">
-        <v>74</v>
+        <v>179</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
@@ -1987,13 +2042,10 @@
         <v>152</v>
       </c>
       <c r="B76" t="s">
-        <v>71</v>
-      </c>
-      <c r="C76" t="s">
-        <v>4</v>
+        <v>28</v>
       </c>
       <c r="D76" t="s">
-        <v>73</v>
+        <v>167</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
@@ -2001,13 +2053,13 @@
         <v>152</v>
       </c>
       <c r="B77" t="s">
-        <v>71</v>
+        <v>28</v>
       </c>
       <c r="C77" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="D77" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
@@ -2015,10 +2067,13 @@
         <v>152</v>
       </c>
       <c r="B78" t="s">
-        <v>27</v>
+        <v>28</v>
+      </c>
+      <c r="C78" t="s">
+        <v>96</v>
       </c>
       <c r="D78" t="s">
-        <v>170</v>
+        <v>67</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
@@ -2026,13 +2081,10 @@
         <v>152</v>
       </c>
       <c r="B79" t="s">
-        <v>27</v>
-      </c>
-      <c r="C79" t="s">
-        <v>0</v>
+        <v>71</v>
       </c>
       <c r="D79" t="s">
-        <v>107</v>
+        <v>168</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
@@ -2040,13 +2092,13 @@
         <v>152</v>
       </c>
       <c r="B80" t="s">
-        <v>27</v>
+        <v>71</v>
       </c>
       <c r="C80" t="s">
-        <v>96</v>
+        <v>1</v>
       </c>
       <c r="D80" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
@@ -2054,10 +2106,13 @@
         <v>152</v>
       </c>
       <c r="B81" t="s">
-        <v>19</v>
+        <v>71</v>
+      </c>
+      <c r="C81" t="s">
+        <v>9</v>
       </c>
       <c r="D81" t="s">
-        <v>172</v>
+        <v>114</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.2">
@@ -2065,13 +2120,13 @@
         <v>152</v>
       </c>
       <c r="B82" t="s">
-        <v>19</v>
+        <v>71</v>
       </c>
       <c r="C82" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D82" t="s">
-        <v>39</v>
+        <v>74</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.2">
@@ -2079,13 +2134,13 @@
         <v>152</v>
       </c>
       <c r="B83" t="s">
-        <v>19</v>
+        <v>71</v>
       </c>
       <c r="C83" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D83" t="s">
-        <v>57</v>
+        <v>73</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.2">
@@ -2093,13 +2148,13 @@
         <v>152</v>
       </c>
       <c r="B84" t="s">
-        <v>19</v>
+        <v>71</v>
       </c>
       <c r="C84" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D84" t="s">
-        <v>38</v>
+        <v>76</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.2">
@@ -2107,10 +2162,10 @@
         <v>152</v>
       </c>
       <c r="B85" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="D85" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.2">
@@ -2118,13 +2173,13 @@
         <v>152</v>
       </c>
       <c r="B86" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="C86" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D86" t="s">
-        <v>51</v>
+        <v>107</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.2">
@@ -2132,13 +2187,13 @@
         <v>152</v>
       </c>
       <c r="B87" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="C87" t="s">
-        <v>0</v>
+        <v>96</v>
       </c>
       <c r="D87" t="s">
-        <v>52</v>
+        <v>67</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.2">
@@ -2146,13 +2201,10 @@
         <v>152</v>
       </c>
       <c r="B88" t="s">
-        <v>20</v>
-      </c>
-      <c r="C88" t="s">
-        <v>75</v>
+        <v>19</v>
       </c>
       <c r="D88" t="s">
-        <v>53</v>
+        <v>172</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.2">
@@ -2160,13 +2212,13 @@
         <v>152</v>
       </c>
       <c r="B89" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C89" t="s">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="D89" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.2">
@@ -2174,10 +2226,13 @@
         <v>152</v>
       </c>
       <c r="B90" t="s">
-        <v>21</v>
+        <v>19</v>
+      </c>
+      <c r="C90" t="s">
+        <v>0</v>
       </c>
       <c r="D90" t="s">
-        <v>174</v>
+        <v>57</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.2">
@@ -2185,13 +2240,13 @@
         <v>152</v>
       </c>
       <c r="B91" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C91" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D91" t="s">
-        <v>65</v>
+        <v>181</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.2">
@@ -2199,13 +2254,13 @@
         <v>152</v>
       </c>
       <c r="B92" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C92" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D92" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.2">
@@ -2213,13 +2268,10 @@
         <v>152</v>
       </c>
       <c r="B93" t="s">
-        <v>21</v>
-      </c>
-      <c r="C93" t="s">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="D93" t="s">
-        <v>58</v>
+        <v>173</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.2">
@@ -2227,13 +2279,13 @@
         <v>152</v>
       </c>
       <c r="B94" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C94" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D94" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.2">
@@ -2241,13 +2293,13 @@
         <v>152</v>
       </c>
       <c r="B95" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C95" t="s">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="D95" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.2">
@@ -2255,13 +2307,13 @@
         <v>152</v>
       </c>
       <c r="B96" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C96" t="s">
-        <v>23</v>
+        <v>75</v>
       </c>
       <c r="D96" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.2">
@@ -2269,13 +2321,13 @@
         <v>152</v>
       </c>
       <c r="B97" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C97" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D97" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.2">
@@ -2285,192 +2337,198 @@
       <c r="B98" t="s">
         <v>21</v>
       </c>
-      <c r="C98" t="s">
-        <v>7</v>
-      </c>
       <c r="D98" t="s">
-        <v>77</v>
+        <v>174</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>154</v>
+        <v>152</v>
+      </c>
+      <c r="B99" t="s">
+        <v>21</v>
+      </c>
+      <c r="C99" t="s">
+        <v>2</v>
       </c>
       <c r="D99" t="s">
-        <v>155</v>
+        <v>65</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B100" t="s">
-        <v>81</v>
+        <v>21</v>
+      </c>
+      <c r="C100" t="s">
+        <v>1</v>
       </c>
       <c r="D100" t="s">
-        <v>160</v>
+        <v>44</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B101" t="s">
-        <v>81</v>
+        <v>21</v>
       </c>
       <c r="C101" t="s">
-        <v>83</v>
+        <v>0</v>
       </c>
       <c r="D101" t="s">
-        <v>85</v>
+        <v>58</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B102" t="s">
-        <v>81</v>
+        <v>21</v>
       </c>
       <c r="C102" t="s">
-        <v>84</v>
+        <v>4</v>
       </c>
       <c r="D102" t="s">
-        <v>92</v>
+        <v>40</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B103" t="s">
-        <v>81</v>
+        <v>21</v>
       </c>
       <c r="C103" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="D103" t="s">
-        <v>82</v>
+        <v>41</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B104" t="s">
-        <v>115</v>
+        <v>21</v>
+      </c>
+      <c r="C104" t="s">
+        <v>23</v>
       </c>
       <c r="D104" t="s">
-        <v>162</v>
+        <v>42</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B105" t="s">
-        <v>115</v>
+        <v>21</v>
       </c>
       <c r="C105" t="s">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="D105" t="s">
-        <v>130</v>
+        <v>43</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B106" t="s">
-        <v>115</v>
+        <v>21</v>
       </c>
       <c r="C106" t="s">
-        <v>116</v>
+        <v>7</v>
       </c>
       <c r="D106" t="s">
-        <v>132</v>
+        <v>77</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B107" t="s">
-        <v>86</v>
+        <v>21</v>
+      </c>
+      <c r="C107" s="1" t="s">
+        <v>182</v>
       </c>
       <c r="D107" t="s">
-        <v>166</v>
+        <v>184</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B108" t="s">
-        <v>86</v>
-      </c>
-      <c r="C108" t="s">
-        <v>88</v>
+        <v>21</v>
+      </c>
+      <c r="C108" s="1" t="s">
+        <v>135</v>
       </c>
       <c r="D108" t="s">
-        <v>89</v>
+        <v>185</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B109" t="s">
-        <v>86</v>
-      </c>
-      <c r="C109" t="s">
-        <v>83</v>
+        <v>21</v>
+      </c>
+      <c r="C109" s="1" t="s">
+        <v>136</v>
       </c>
       <c r="D109" t="s">
-        <v>90</v>
+        <v>186</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B110" t="s">
-        <v>86</v>
-      </c>
-      <c r="C110" t="s">
-        <v>84</v>
+        <v>21</v>
+      </c>
+      <c r="C110" s="1" t="s">
+        <v>183</v>
       </c>
       <c r="D110" t="s">
-        <v>91</v>
+        <v>187</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B111" t="s">
-        <v>86</v>
-      </c>
-      <c r="C111" t="s">
-        <v>0</v>
+        <v>21</v>
+      </c>
+      <c r="C111" s="1" t="s">
+        <v>175</v>
       </c>
       <c r="D111" t="s">
-        <v>87</v>
+        <v>180</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>154</v>
       </c>
-      <c r="B112" t="s">
-        <v>86</v>
-      </c>
-      <c r="C112" t="s">
-        <v>93</v>
-      </c>
       <c r="D112" t="s">
-        <v>94</v>
+        <v>155</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.2">
@@ -2478,10 +2536,10 @@
         <v>154</v>
       </c>
       <c r="B113" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="D113" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.2">
@@ -2489,13 +2547,13 @@
         <v>154</v>
       </c>
       <c r="B114" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="C114" t="s">
-        <v>0</v>
+        <v>83</v>
       </c>
       <c r="D114" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.2">
@@ -2503,13 +2561,13 @@
         <v>154</v>
       </c>
       <c r="B115" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="C115" t="s">
-        <v>20</v>
+        <v>84</v>
       </c>
       <c r="D115" t="s">
-        <v>80</v>
+        <v>92</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.2">
@@ -2517,10 +2575,13 @@
         <v>154</v>
       </c>
       <c r="B116" t="s">
-        <v>117</v>
+        <v>81</v>
+      </c>
+      <c r="C116" t="s">
+        <v>0</v>
       </c>
       <c r="D116" t="s">
-        <v>171</v>
+        <v>82</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.2">
@@ -2528,13 +2589,13 @@
         <v>154</v>
       </c>
       <c r="B117" t="s">
-        <v>117</v>
+        <v>81</v>
       </c>
       <c r="C117" t="s">
-        <v>118</v>
+        <v>93</v>
       </c>
       <c r="D117" t="s">
-        <v>121</v>
+        <v>188</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.2">
@@ -2542,13 +2603,10 @@
         <v>154</v>
       </c>
       <c r="B118" t="s">
-        <v>117</v>
-      </c>
-      <c r="C118" t="s">
-        <v>0</v>
+        <v>115</v>
       </c>
       <c r="D118" t="s">
-        <v>120</v>
+        <v>162</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.2">
@@ -2556,13 +2614,13 @@
         <v>154</v>
       </c>
       <c r="B119" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C119" t="s">
-        <v>119</v>
+        <v>0</v>
       </c>
       <c r="D119" t="s">
-        <v>122</v>
+        <v>130</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.2">
@@ -2570,16 +2628,204 @@
         <v>154</v>
       </c>
       <c r="B120" t="s">
+        <v>115</v>
+      </c>
+      <c r="C120" t="s">
+        <v>116</v>
+      </c>
+      <c r="D120" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A121" t="s">
+        <v>154</v>
+      </c>
+      <c r="B121" t="s">
+        <v>86</v>
+      </c>
+      <c r="D121" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A122" t="s">
+        <v>154</v>
+      </c>
+      <c r="B122" t="s">
+        <v>86</v>
+      </c>
+      <c r="C122" t="s">
+        <v>88</v>
+      </c>
+      <c r="D122" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A123" t="s">
+        <v>154</v>
+      </c>
+      <c r="B123" t="s">
+        <v>86</v>
+      </c>
+      <c r="C123" t="s">
+        <v>83</v>
+      </c>
+      <c r="D123" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A124" t="s">
+        <v>154</v>
+      </c>
+      <c r="B124" t="s">
+        <v>86</v>
+      </c>
+      <c r="C124" t="s">
+        <v>84</v>
+      </c>
+      <c r="D124" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A125" t="s">
+        <v>154</v>
+      </c>
+      <c r="B125" t="s">
+        <v>86</v>
+      </c>
+      <c r="C125" t="s">
+        <v>0</v>
+      </c>
+      <c r="D125" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A126" t="s">
+        <v>154</v>
+      </c>
+      <c r="B126" t="s">
+        <v>86</v>
+      </c>
+      <c r="C126" t="s">
+        <v>93</v>
+      </c>
+      <c r="D126" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A127" t="s">
+        <v>154</v>
+      </c>
+      <c r="B127" t="s">
+        <v>78</v>
+      </c>
+      <c r="D127" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A128" t="s">
+        <v>154</v>
+      </c>
+      <c r="B128" t="s">
+        <v>78</v>
+      </c>
+      <c r="C128" t="s">
+        <v>0</v>
+      </c>
+      <c r="D128" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A129" t="s">
+        <v>154</v>
+      </c>
+      <c r="B129" t="s">
+        <v>78</v>
+      </c>
+      <c r="C129" t="s">
+        <v>20</v>
+      </c>
+      <c r="D129" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A130" t="s">
+        <v>154</v>
+      </c>
+      <c r="B130" t="s">
         <v>117</v>
       </c>
-      <c r="C120" t="s">
+      <c r="D130" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A131" t="s">
+        <v>154</v>
+      </c>
+      <c r="B131" t="s">
+        <v>117</v>
+      </c>
+      <c r="C131" t="s">
+        <v>118</v>
+      </c>
+      <c r="D131" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A132" t="s">
+        <v>154</v>
+      </c>
+      <c r="B132" t="s">
+        <v>117</v>
+      </c>
+      <c r="C132" t="s">
+        <v>0</v>
+      </c>
+      <c r="D132" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A133" t="s">
+        <v>154</v>
+      </c>
+      <c r="B133" t="s">
+        <v>117</v>
+      </c>
+      <c r="C133" t="s">
+        <v>119</v>
+      </c>
+      <c r="D133" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A134" t="s">
+        <v>154</v>
+      </c>
+      <c r="B134" t="s">
+        <v>117</v>
+      </c>
+      <c r="C134" t="s">
         <v>93</v>
       </c>
-      <c r="D120" t="s">
+      <c r="D134" t="s">
         <v>123</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>

</xml_diff>

<commit_message>
changed : harmonize variable naming in search_history indexdb data
</commit_message>
<xml_diff>
--- a/public/data/db_source/__meta_schema__.xlsx
+++ b/public/data/db_source/__meta_schema__.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10916"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11027"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bassim/code/datannur/datannur_dev/public/data/db_source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4638EFDA-B734-1943-A292-852528CDDEDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{387B9C73-2628-E942-88B8-24A64BDB470A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2680" yWindow="500" windowWidth="26120" windowHeight="17500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="513" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="513" uniqueCount="187">
   <si>
     <t>id</t>
   </si>
@@ -390,12 +390,6 @@
   </si>
   <si>
     <t>search_history</t>
-  </si>
-  <si>
-    <t>entity_name</t>
-  </si>
-  <si>
-    <t>item_id</t>
   </si>
   <si>
     <t>clé primaire de la recherche</t>
@@ -644,9 +638,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1006,7 +999,7 @@
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" zoomScale="125" zoomScaleNormal="140" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A106" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D119" sqref="D119"/>
+      <selection pane="bottomLeft" activeCell="D129" sqref="D129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1033,26 +1026,26 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D2" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B3" t="s">
         <v>17</v>
       </c>
       <c r="D3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B4" t="s">
         <v>17</v>
@@ -1066,7 +1059,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B5" t="s">
         <v>17</v>
@@ -1080,7 +1073,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B6" t="s">
         <v>17</v>
@@ -1094,18 +1087,18 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B7" t="s">
         <v>25</v>
       </c>
       <c r="D7" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B8" t="s">
         <v>25</v>
@@ -1119,7 +1112,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B9" t="s">
         <v>25</v>
@@ -1133,32 +1126,32 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B10" t="s">
         <v>8</v>
       </c>
       <c r="D10" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B11" t="s">
         <v>8</v>
       </c>
       <c r="C11" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D11" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B12" t="s">
         <v>8</v>
@@ -1167,12 +1160,12 @@
         <v>102</v>
       </c>
       <c r="D12" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B13" t="s">
         <v>8</v>
@@ -1186,21 +1179,21 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B14" t="s">
         <v>8</v>
       </c>
       <c r="C14" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D14" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B15" t="s">
         <v>8</v>
@@ -1214,7 +1207,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B16" t="s">
         <v>8</v>
@@ -1228,7 +1221,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B17" t="s">
         <v>8</v>
@@ -1242,7 +1235,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B18" t="s">
         <v>8</v>
@@ -1256,7 +1249,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B19" t="s">
         <v>8</v>
@@ -1265,12 +1258,12 @@
         <v>109</v>
       </c>
       <c r="D19" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B20" t="s">
         <v>8</v>
@@ -1284,7 +1277,7 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B21" t="s">
         <v>8</v>
@@ -1298,7 +1291,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B22" t="s">
         <v>8</v>
@@ -1312,7 +1305,7 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B23" t="s">
         <v>8</v>
@@ -1326,7 +1319,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B24" t="s">
         <v>8</v>
@@ -1340,21 +1333,21 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B25" t="s">
         <v>8</v>
       </c>
       <c r="C25" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D25" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B26" t="s">
         <v>8</v>
@@ -1368,7 +1361,7 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B27" t="s">
         <v>8</v>
@@ -1382,46 +1375,46 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B28" t="s">
         <v>8</v>
       </c>
       <c r="C28" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D28" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B29" t="s">
         <v>8</v>
       </c>
       <c r="C29" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D29" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B30" t="s">
         <v>110</v>
       </c>
       <c r="D30" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B31" t="s">
         <v>110</v>
@@ -1435,7 +1428,7 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B32" t="s">
         <v>110</v>
@@ -1444,12 +1437,12 @@
         <v>83</v>
       </c>
       <c r="D32" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B33" t="s">
         <v>110</v>
@@ -1463,7 +1456,7 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B34" t="s">
         <v>110</v>
@@ -1472,12 +1465,12 @@
         <v>0</v>
       </c>
       <c r="D34" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B35" t="s">
         <v>110</v>
@@ -1491,7 +1484,7 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B36" t="s">
         <v>110</v>
@@ -1500,12 +1493,12 @@
         <v>4</v>
       </c>
       <c r="D36" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B37" t="s">
         <v>110</v>
@@ -1514,12 +1507,12 @@
         <v>111</v>
       </c>
       <c r="D37" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B38" t="s">
         <v>110</v>
@@ -1528,37 +1521,37 @@
         <v>7</v>
       </c>
       <c r="D38" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B39" t="s">
         <v>110</v>
       </c>
       <c r="C39" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D39" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B40" t="s">
         <v>112</v>
       </c>
       <c r="D40" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B41" t="s">
         <v>112</v>
@@ -1567,12 +1560,12 @@
         <v>0</v>
       </c>
       <c r="D41" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B42" t="s">
         <v>112</v>
@@ -1581,37 +1574,37 @@
         <v>4</v>
       </c>
       <c r="D42" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B43" t="s">
         <v>26</v>
       </c>
       <c r="D43" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B44" t="s">
         <v>26</v>
       </c>
       <c r="C44" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D44" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B45" t="s">
         <v>26</v>
@@ -1625,7 +1618,7 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B46" t="s">
         <v>26</v>
@@ -1639,35 +1632,35 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B47" t="s">
         <v>26</v>
       </c>
       <c r="C47" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D47" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B48" t="s">
         <v>26</v>
       </c>
       <c r="C48" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D48" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B49" t="s">
         <v>26</v>
@@ -1681,7 +1674,7 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B50" t="s">
         <v>26</v>
@@ -1690,12 +1683,12 @@
         <v>15</v>
       </c>
       <c r="D50" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B51" t="s">
         <v>26</v>
@@ -1704,12 +1697,12 @@
         <v>109</v>
       </c>
       <c r="D51" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B52" t="s">
         <v>26</v>
@@ -1723,21 +1716,21 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B53" t="s">
         <v>26</v>
       </c>
       <c r="C53" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D53" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B54" t="s">
         <v>26</v>
@@ -1751,7 +1744,7 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B55" t="s">
         <v>26</v>
@@ -1765,7 +1758,7 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B56" t="s">
         <v>26</v>
@@ -1779,7 +1772,7 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B57" t="s">
         <v>26</v>
@@ -1793,21 +1786,21 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B58" t="s">
         <v>26</v>
       </c>
       <c r="C58" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D58" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B59" t="s">
         <v>26</v>
@@ -1821,7 +1814,7 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B60" t="s">
         <v>26</v>
@@ -1830,51 +1823,51 @@
         <v>16</v>
       </c>
       <c r="D60" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B61" t="s">
         <v>26</v>
       </c>
       <c r="C61" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D61" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B62" t="s">
         <v>26</v>
       </c>
       <c r="C62" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D62" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B63" t="s">
         <v>113</v>
       </c>
       <c r="D63" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B64" t="s">
         <v>113</v>
@@ -1883,12 +1876,12 @@
         <v>0</v>
       </c>
       <c r="D64" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B65" t="s">
         <v>113</v>
@@ -1897,23 +1890,23 @@
         <v>20</v>
       </c>
       <c r="D65" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B66" t="s">
         <v>95</v>
       </c>
       <c r="D66" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B67" t="s">
         <v>95</v>
@@ -1927,7 +1920,7 @@
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B68" t="s">
         <v>95</v>
@@ -1941,7 +1934,7 @@
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B69" t="s">
         <v>95</v>
@@ -1955,7 +1948,7 @@
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B70" t="s">
         <v>95</v>
@@ -1969,7 +1962,7 @@
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B71" t="s">
         <v>95</v>
@@ -1983,7 +1976,7 @@
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B72" t="s">
         <v>95</v>
@@ -1997,7 +1990,7 @@
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B73" t="s">
         <v>95</v>
@@ -2011,46 +2004,46 @@
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B74" t="s">
         <v>95</v>
       </c>
       <c r="C74" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D74" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B75" t="s">
         <v>95</v>
       </c>
       <c r="C75" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D75" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B76" t="s">
         <v>28</v>
       </c>
       <c r="D76" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B77" t="s">
         <v>28</v>
@@ -2064,7 +2057,7 @@
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B78" t="s">
         <v>28</v>
@@ -2078,18 +2071,18 @@
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B79" t="s">
         <v>71</v>
       </c>
       <c r="D79" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B80" t="s">
         <v>71</v>
@@ -2103,7 +2096,7 @@
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B81" t="s">
         <v>71</v>
@@ -2117,7 +2110,7 @@
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B82" t="s">
         <v>71</v>
@@ -2131,7 +2124,7 @@
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B83" t="s">
         <v>71</v>
@@ -2145,7 +2138,7 @@
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B84" t="s">
         <v>71</v>
@@ -2159,18 +2152,18 @@
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B85" t="s">
         <v>27</v>
       </c>
       <c r="D85" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B86" t="s">
         <v>27</v>
@@ -2184,7 +2177,7 @@
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B87" t="s">
         <v>27</v>
@@ -2198,18 +2191,18 @@
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B88" t="s">
         <v>19</v>
       </c>
       <c r="D88" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B89" t="s">
         <v>19</v>
@@ -2223,7 +2216,7 @@
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B90" t="s">
         <v>19</v>
@@ -2237,7 +2230,7 @@
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B91" t="s">
         <v>19</v>
@@ -2246,12 +2239,12 @@
         <v>3</v>
       </c>
       <c r="D91" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B92" t="s">
         <v>19</v>
@@ -2265,18 +2258,18 @@
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B93" t="s">
         <v>20</v>
       </c>
       <c r="D93" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B94" t="s">
         <v>20</v>
@@ -2290,7 +2283,7 @@
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B95" t="s">
         <v>20</v>
@@ -2304,7 +2297,7 @@
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B96" t="s">
         <v>20</v>
@@ -2318,7 +2311,7 @@
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B97" t="s">
         <v>20</v>
@@ -2332,18 +2325,18 @@
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B98" t="s">
         <v>21</v>
       </c>
       <c r="D98" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B99" t="s">
         <v>21</v>
@@ -2357,7 +2350,7 @@
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B100" t="s">
         <v>21</v>
@@ -2371,7 +2364,7 @@
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B101" t="s">
         <v>21</v>
@@ -2385,7 +2378,7 @@
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B102" t="s">
         <v>21</v>
@@ -2399,7 +2392,7 @@
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B103" t="s">
         <v>21</v>
@@ -2413,7 +2406,7 @@
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B104" t="s">
         <v>21</v>
@@ -2427,7 +2420,7 @@
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B105" t="s">
         <v>21</v>
@@ -2441,7 +2434,7 @@
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B106" t="s">
         <v>21</v>
@@ -2455,96 +2448,96 @@
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B107" t="s">
         <v>21</v>
       </c>
-      <c r="C107" s="1" t="s">
+      <c r="C107" t="s">
+        <v>180</v>
+      </c>
+      <c r="D107" t="s">
         <v>182</v>
-      </c>
-      <c r="D107" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B108" t="s">
         <v>21</v>
       </c>
-      <c r="C108" s="1" t="s">
-        <v>135</v>
+      <c r="C108" t="s">
+        <v>133</v>
       </c>
       <c r="D108" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B109" t="s">
         <v>21</v>
       </c>
-      <c r="C109" s="1" t="s">
-        <v>136</v>
+      <c r="C109" t="s">
+        <v>134</v>
       </c>
       <c r="D109" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B110" t="s">
         <v>21</v>
       </c>
-      <c r="C110" s="1" t="s">
-        <v>183</v>
+      <c r="C110" t="s">
+        <v>181</v>
       </c>
       <c r="D110" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B111" t="s">
         <v>21</v>
       </c>
-      <c r="C111" s="1" t="s">
-        <v>175</v>
+      <c r="C111" t="s">
+        <v>173</v>
       </c>
       <c r="D111" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D112" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B113" t="s">
         <v>81</v>
       </c>
       <c r="D113" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B114" t="s">
         <v>81</v>
@@ -2558,7 +2551,7 @@
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B115" t="s">
         <v>81</v>
@@ -2572,7 +2565,7 @@
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B116" t="s">
         <v>81</v>
@@ -2586,7 +2579,7 @@
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B117" t="s">
         <v>81</v>
@@ -2595,23 +2588,23 @@
         <v>93</v>
       </c>
       <c r="D117" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B118" t="s">
         <v>115</v>
       </c>
       <c r="D118" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B119" t="s">
         <v>115</v>
@@ -2620,12 +2613,12 @@
         <v>0</v>
       </c>
       <c r="D119" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B120" t="s">
         <v>115</v>
@@ -2634,23 +2627,23 @@
         <v>116</v>
       </c>
       <c r="D120" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B121" t="s">
         <v>86</v>
       </c>
       <c r="D121" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B122" t="s">
         <v>86</v>
@@ -2664,7 +2657,7 @@
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B123" t="s">
         <v>86</v>
@@ -2678,7 +2671,7 @@
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B124" t="s">
         <v>86</v>
@@ -2692,7 +2685,7 @@
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B125" t="s">
         <v>86</v>
@@ -2706,7 +2699,7 @@
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B126" t="s">
         <v>86</v>
@@ -2720,18 +2713,18 @@
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B127" t="s">
         <v>78</v>
       </c>
       <c r="D127" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B128" t="s">
         <v>78</v>
@@ -2745,7 +2738,7 @@
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B129" t="s">
         <v>78</v>
@@ -2759,38 +2752,38 @@
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B130" t="s">
         <v>117</v>
       </c>
       <c r="D130" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B131" t="s">
         <v>117</v>
       </c>
       <c r="C131" t="s">
-        <v>118</v>
+        <v>83</v>
       </c>
       <c r="D131" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B132" t="s">
         <v>117</v>
       </c>
       <c r="C132" t="s">
-        <v>0</v>
+        <v>84</v>
       </c>
       <c r="D132" t="s">
         <v>120</v>
@@ -2798,21 +2791,21 @@
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B133" t="s">
         <v>117</v>
       </c>
       <c r="C133" t="s">
-        <v>119</v>
+        <v>0</v>
       </c>
       <c r="D133" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B134" t="s">
         <v>117</v>
@@ -2821,7 +2814,7 @@
         <v>93</v>
       </c>
       <c r="D134" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added : processing of history changes in jsonjsdb_editor
</commit_message>
<xml_diff>
--- a/public/data/db_source/__meta_schema__.xlsx
+++ b/public/data/db_source/__meta_schema__.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11027"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11207"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bassim/code/datannur/datannur_dev/public/data/db_source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{387B9C73-2628-E942-88B8-24A64BDB470A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87B4EFF7-65D2-E648-B31B-A5377CE6D88B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2680" yWindow="500" windowWidth="26120" windowHeight="17500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="513" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="198">
   <si>
     <t>id</t>
   </si>
@@ -597,6 +597,39 @@
   </si>
   <si>
     <t>timestamp unix de l'ajout du favori</t>
+  </si>
+  <si>
+    <t>history</t>
+  </si>
+  <si>
+    <t>old_value</t>
+  </si>
+  <si>
+    <t>new_value</t>
+  </si>
+  <si>
+    <t>type de changement (ajout, suppression ou modification)</t>
+  </si>
+  <si>
+    <t>timestamp unix du changement</t>
+  </si>
+  <si>
+    <t>Historique des changements dans les métadonnées</t>
+  </si>
+  <si>
+    <t>nom de l'entité concernée par le changement</t>
+  </si>
+  <si>
+    <t>id de l'élement concernée par le changement</t>
+  </si>
+  <si>
+    <t>variable concernée par la modification</t>
+  </si>
+  <si>
+    <t>valeur avant modification</t>
+  </si>
+  <si>
+    <t>valeur après modification</t>
   </si>
 </sst>
 </file>
@@ -658,10 +691,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{CC52189E-6718-7640-A09D-3E13A3AE1ED2}" name="Tableau3" displayName="Tableau3" ref="A1:D134" totalsRowShown="0">
-  <autoFilter ref="A1:D134" xr:uid="{CC52189E-6718-7640-A09D-3E13A3AE1ED2}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D134">
-    <sortCondition ref="A1:A134"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{CC52189E-6718-7640-A09D-3E13A3AE1ED2}" name="Tableau3" displayName="Tableau3" ref="A1:D142" totalsRowShown="0">
+  <autoFilter ref="A1:D142" xr:uid="{CC52189E-6718-7640-A09D-3E13A3AE1ED2}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D142">
+    <sortCondition ref="A1:A142"/>
   </sortState>
   <tableColumns count="4">
     <tableColumn id="4" xr3:uid="{D4AE5F0B-EFF7-F144-B9F0-6F582D88D1B3}" name="folder"/>
@@ -995,11 +1028,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D134"/>
+  <dimension ref="A1:D142"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" zoomScale="125" zoomScaleNormal="140" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A106" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D129" sqref="D129"/>
+      <pane ySplit="1" topLeftCell="A52" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D72" sqref="D72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1859,10 +1892,10 @@
         <v>150</v>
       </c>
       <c r="B63" t="s">
-        <v>113</v>
+        <v>187</v>
       </c>
       <c r="D63" t="s">
-        <v>162</v>
+        <v>192</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
@@ -1870,13 +1903,13 @@
         <v>150</v>
       </c>
       <c r="B64" t="s">
-        <v>113</v>
+        <v>187</v>
       </c>
       <c r="C64" t="s">
-        <v>0</v>
+        <v>93</v>
       </c>
       <c r="D64" t="s">
-        <v>131</v>
+        <v>191</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
@@ -1884,13 +1917,13 @@
         <v>150</v>
       </c>
       <c r="B65" t="s">
-        <v>113</v>
+        <v>187</v>
       </c>
       <c r="C65" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="D65" t="s">
-        <v>132</v>
+        <v>190</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
@@ -1898,10 +1931,13 @@
         <v>150</v>
       </c>
       <c r="B66" t="s">
-        <v>95</v>
+        <v>187</v>
+      </c>
+      <c r="C66" t="s">
+        <v>83</v>
       </c>
       <c r="D66" t="s">
-        <v>163</v>
+        <v>193</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
@@ -1909,13 +1945,13 @@
         <v>150</v>
       </c>
       <c r="B67" t="s">
-        <v>95</v>
+        <v>187</v>
       </c>
       <c r="C67" t="s">
-        <v>1</v>
+        <v>84</v>
       </c>
       <c r="D67" t="s">
-        <v>6</v>
+        <v>194</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
@@ -1923,13 +1959,13 @@
         <v>150</v>
       </c>
       <c r="B68" t="s">
-        <v>95</v>
+        <v>187</v>
       </c>
       <c r="C68" t="s">
-        <v>97</v>
+        <v>21</v>
       </c>
       <c r="D68" t="s">
-        <v>99</v>
+        <v>195</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
@@ -1937,13 +1973,13 @@
         <v>150</v>
       </c>
       <c r="B69" t="s">
-        <v>95</v>
+        <v>187</v>
       </c>
       <c r="C69" t="s">
-        <v>0</v>
+        <v>188</v>
       </c>
       <c r="D69" t="s">
-        <v>54</v>
+        <v>196</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
@@ -1951,13 +1987,13 @@
         <v>150</v>
       </c>
       <c r="B70" t="s">
-        <v>95</v>
+        <v>187</v>
       </c>
       <c r="C70" t="s">
-        <v>4</v>
+        <v>189</v>
       </c>
       <c r="D70" t="s">
-        <v>5</v>
+        <v>197</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
@@ -1965,13 +2001,10 @@
         <v>150</v>
       </c>
       <c r="B71" t="s">
-        <v>95</v>
-      </c>
-      <c r="C71" t="s">
-        <v>3</v>
+        <v>113</v>
       </c>
       <c r="D71" t="s">
-        <v>70</v>
+        <v>162</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
@@ -1979,13 +2012,13 @@
         <v>150</v>
       </c>
       <c r="B72" t="s">
-        <v>95</v>
+        <v>113</v>
       </c>
       <c r="C72" t="s">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="D72" t="s">
-        <v>49</v>
+        <v>131</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
@@ -1993,13 +2026,13 @@
         <v>150</v>
       </c>
       <c r="B73" t="s">
-        <v>95</v>
+        <v>113</v>
       </c>
       <c r="C73" t="s">
-        <v>98</v>
+        <v>20</v>
       </c>
       <c r="D73" t="s">
-        <v>100</v>
+        <v>132</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
@@ -2009,11 +2042,8 @@
       <c r="B74" t="s">
         <v>95</v>
       </c>
-      <c r="C74" t="s">
-        <v>173</v>
-      </c>
       <c r="D74" t="s">
-        <v>178</v>
+        <v>163</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
@@ -2024,10 +2054,10 @@
         <v>95</v>
       </c>
       <c r="C75" t="s">
-        <v>174</v>
+        <v>1</v>
       </c>
       <c r="D75" t="s">
-        <v>177</v>
+        <v>6</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
@@ -2035,10 +2065,13 @@
         <v>150</v>
       </c>
       <c r="B76" t="s">
-        <v>28</v>
+        <v>95</v>
+      </c>
+      <c r="C76" t="s">
+        <v>97</v>
       </c>
       <c r="D76" t="s">
-        <v>165</v>
+        <v>99</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
@@ -2046,13 +2079,13 @@
         <v>150</v>
       </c>
       <c r="B77" t="s">
-        <v>28</v>
+        <v>95</v>
       </c>
       <c r="C77" t="s">
         <v>0</v>
       </c>
       <c r="D77" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
@@ -2060,13 +2093,13 @@
         <v>150</v>
       </c>
       <c r="B78" t="s">
-        <v>28</v>
+        <v>95</v>
       </c>
       <c r="C78" t="s">
-        <v>96</v>
+        <v>4</v>
       </c>
       <c r="D78" t="s">
-        <v>67</v>
+        <v>5</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
@@ -2074,10 +2107,13 @@
         <v>150</v>
       </c>
       <c r="B79" t="s">
-        <v>71</v>
+        <v>95</v>
+      </c>
+      <c r="C79" t="s">
+        <v>3</v>
       </c>
       <c r="D79" t="s">
-        <v>166</v>
+        <v>70</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
@@ -2085,13 +2121,13 @@
         <v>150</v>
       </c>
       <c r="B80" t="s">
-        <v>71</v>
+        <v>95</v>
       </c>
       <c r="C80" t="s">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="D80" t="s">
-        <v>72</v>
+        <v>49</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
@@ -2099,13 +2135,13 @@
         <v>150</v>
       </c>
       <c r="B81" t="s">
-        <v>71</v>
+        <v>95</v>
       </c>
       <c r="C81" t="s">
-        <v>9</v>
+        <v>98</v>
       </c>
       <c r="D81" t="s">
-        <v>114</v>
+        <v>100</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.2">
@@ -2113,13 +2149,13 @@
         <v>150</v>
       </c>
       <c r="B82" t="s">
-        <v>71</v>
+        <v>95</v>
       </c>
       <c r="C82" t="s">
-        <v>0</v>
+        <v>173</v>
       </c>
       <c r="D82" t="s">
-        <v>74</v>
+        <v>178</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.2">
@@ -2127,13 +2163,13 @@
         <v>150</v>
       </c>
       <c r="B83" t="s">
-        <v>71</v>
+        <v>95</v>
       </c>
       <c r="C83" t="s">
-        <v>4</v>
+        <v>174</v>
       </c>
       <c r="D83" t="s">
-        <v>73</v>
+        <v>177</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.2">
@@ -2141,13 +2177,10 @@
         <v>150</v>
       </c>
       <c r="B84" t="s">
-        <v>71</v>
-      </c>
-      <c r="C84" t="s">
-        <v>7</v>
+        <v>28</v>
       </c>
       <c r="D84" t="s">
-        <v>76</v>
+        <v>165</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.2">
@@ -2155,10 +2188,13 @@
         <v>150</v>
       </c>
       <c r="B85" t="s">
-        <v>27</v>
+        <v>28</v>
+      </c>
+      <c r="C85" t="s">
+        <v>0</v>
       </c>
       <c r="D85" t="s">
-        <v>168</v>
+        <v>61</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.2">
@@ -2166,13 +2202,13 @@
         <v>150</v>
       </c>
       <c r="B86" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C86" t="s">
-        <v>0</v>
+        <v>96</v>
       </c>
       <c r="D86" t="s">
-        <v>107</v>
+        <v>67</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.2">
@@ -2180,13 +2216,10 @@
         <v>150</v>
       </c>
       <c r="B87" t="s">
-        <v>27</v>
-      </c>
-      <c r="C87" t="s">
-        <v>96</v>
+        <v>71</v>
       </c>
       <c r="D87" t="s">
-        <v>67</v>
+        <v>166</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.2">
@@ -2194,10 +2227,13 @@
         <v>150</v>
       </c>
       <c r="B88" t="s">
-        <v>19</v>
+        <v>71</v>
+      </c>
+      <c r="C88" t="s">
+        <v>1</v>
       </c>
       <c r="D88" t="s">
-        <v>170</v>
+        <v>72</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.2">
@@ -2205,13 +2241,13 @@
         <v>150</v>
       </c>
       <c r="B89" t="s">
-        <v>19</v>
+        <v>71</v>
       </c>
       <c r="C89" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="D89" t="s">
-        <v>39</v>
+        <v>114</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.2">
@@ -2219,13 +2255,13 @@
         <v>150</v>
       </c>
       <c r="B90" t="s">
-        <v>19</v>
+        <v>71</v>
       </c>
       <c r="C90" t="s">
         <v>0</v>
       </c>
       <c r="D90" t="s">
-        <v>57</v>
+        <v>74</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.2">
@@ -2233,13 +2269,13 @@
         <v>150</v>
       </c>
       <c r="B91" t="s">
-        <v>19</v>
+        <v>71</v>
       </c>
       <c r="C91" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D91" t="s">
-        <v>179</v>
+        <v>73</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.2">
@@ -2247,13 +2283,13 @@
         <v>150</v>
       </c>
       <c r="B92" t="s">
-        <v>19</v>
+        <v>71</v>
       </c>
       <c r="C92" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D92" t="s">
-        <v>38</v>
+        <v>76</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.2">
@@ -2261,10 +2297,10 @@
         <v>150</v>
       </c>
       <c r="B93" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="D93" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.2">
@@ -2272,13 +2308,13 @@
         <v>150</v>
       </c>
       <c r="B94" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="C94" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D94" t="s">
-        <v>51</v>
+        <v>107</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.2">
@@ -2286,13 +2322,13 @@
         <v>150</v>
       </c>
       <c r="B95" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="C95" t="s">
-        <v>0</v>
+        <v>96</v>
       </c>
       <c r="D95" t="s">
-        <v>52</v>
+        <v>67</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.2">
@@ -2300,13 +2336,10 @@
         <v>150</v>
       </c>
       <c r="B96" t="s">
-        <v>20</v>
-      </c>
-      <c r="C96" t="s">
-        <v>75</v>
+        <v>19</v>
       </c>
       <c r="D96" t="s">
-        <v>53</v>
+        <v>170</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.2">
@@ -2314,13 +2347,13 @@
         <v>150</v>
       </c>
       <c r="B97" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C97" t="s">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="D97" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.2">
@@ -2328,10 +2361,13 @@
         <v>150</v>
       </c>
       <c r="B98" t="s">
-        <v>21</v>
+        <v>19</v>
+      </c>
+      <c r="C98" t="s">
+        <v>0</v>
       </c>
       <c r="D98" t="s">
-        <v>172</v>
+        <v>57</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.2">
@@ -2339,13 +2375,13 @@
         <v>150</v>
       </c>
       <c r="B99" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C99" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D99" t="s">
-        <v>65</v>
+        <v>179</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.2">
@@ -2353,13 +2389,13 @@
         <v>150</v>
       </c>
       <c r="B100" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C100" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D100" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.2">
@@ -2367,13 +2403,10 @@
         <v>150</v>
       </c>
       <c r="B101" t="s">
-        <v>21</v>
-      </c>
-      <c r="C101" t="s">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="D101" t="s">
-        <v>58</v>
+        <v>171</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.2">
@@ -2381,13 +2414,13 @@
         <v>150</v>
       </c>
       <c r="B102" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C102" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D102" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.2">
@@ -2395,13 +2428,13 @@
         <v>150</v>
       </c>
       <c r="B103" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C103" t="s">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="D103" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.2">
@@ -2409,13 +2442,13 @@
         <v>150</v>
       </c>
       <c r="B104" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C104" t="s">
-        <v>23</v>
+        <v>75</v>
       </c>
       <c r="D104" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.2">
@@ -2423,13 +2456,13 @@
         <v>150</v>
       </c>
       <c r="B105" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C105" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D105" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.2">
@@ -2439,11 +2472,8 @@
       <c r="B106" t="s">
         <v>21</v>
       </c>
-      <c r="C106" t="s">
-        <v>7</v>
-      </c>
       <c r="D106" t="s">
-        <v>77</v>
+        <v>172</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.2">
@@ -2454,10 +2484,10 @@
         <v>21</v>
       </c>
       <c r="C107" t="s">
-        <v>180</v>
+        <v>2</v>
       </c>
       <c r="D107" t="s">
-        <v>182</v>
+        <v>65</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.2">
@@ -2468,10 +2498,10 @@
         <v>21</v>
       </c>
       <c r="C108" t="s">
-        <v>133</v>
+        <v>1</v>
       </c>
       <c r="D108" t="s">
-        <v>183</v>
+        <v>44</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.2">
@@ -2482,10 +2512,10 @@
         <v>21</v>
       </c>
       <c r="C109" t="s">
-        <v>134</v>
+        <v>0</v>
       </c>
       <c r="D109" t="s">
-        <v>184</v>
+        <v>58</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.2">
@@ -2496,10 +2526,10 @@
         <v>21</v>
       </c>
       <c r="C110" t="s">
-        <v>181</v>
+        <v>4</v>
       </c>
       <c r="D110" t="s">
-        <v>185</v>
+        <v>40</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.2">
@@ -2510,124 +2540,130 @@
         <v>21</v>
       </c>
       <c r="C111" t="s">
-        <v>173</v>
+        <v>22</v>
       </c>
       <c r="D111" t="s">
-        <v>178</v>
+        <v>41</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>152</v>
+        <v>150</v>
+      </c>
+      <c r="B112" t="s">
+        <v>21</v>
+      </c>
+      <c r="C112" t="s">
+        <v>23</v>
       </c>
       <c r="D112" t="s">
-        <v>153</v>
+        <v>42</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B113" t="s">
-        <v>81</v>
+        <v>21</v>
+      </c>
+      <c r="C113" t="s">
+        <v>24</v>
       </c>
       <c r="D113" t="s">
-        <v>158</v>
+        <v>43</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B114" t="s">
-        <v>81</v>
+        <v>21</v>
       </c>
       <c r="C114" t="s">
-        <v>83</v>
+        <v>7</v>
       </c>
       <c r="D114" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B115" t="s">
-        <v>81</v>
+        <v>21</v>
       </c>
       <c r="C115" t="s">
-        <v>84</v>
+        <v>180</v>
       </c>
       <c r="D115" t="s">
-        <v>92</v>
+        <v>182</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B116" t="s">
-        <v>81</v>
+        <v>21</v>
       </c>
       <c r="C116" t="s">
-        <v>0</v>
+        <v>133</v>
       </c>
       <c r="D116" t="s">
-        <v>82</v>
+        <v>183</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B117" t="s">
-        <v>81</v>
+        <v>21</v>
       </c>
       <c r="C117" t="s">
-        <v>93</v>
+        <v>134</v>
       </c>
       <c r="D117" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B118" t="s">
-        <v>115</v>
+        <v>21</v>
+      </c>
+      <c r="C118" t="s">
+        <v>181</v>
       </c>
       <c r="D118" t="s">
-        <v>160</v>
+        <v>185</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B119" t="s">
-        <v>115</v>
+        <v>21</v>
       </c>
       <c r="C119" t="s">
-        <v>0</v>
+        <v>173</v>
       </c>
       <c r="D119" t="s">
-        <v>128</v>
+        <v>178</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>152</v>
       </c>
-      <c r="B120" t="s">
-        <v>115</v>
-      </c>
-      <c r="C120" t="s">
-        <v>116</v>
-      </c>
       <c r="D120" t="s">
-        <v>130</v>
+        <v>153</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.2">
@@ -2635,10 +2671,10 @@
         <v>152</v>
       </c>
       <c r="B121" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="D121" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.2">
@@ -2646,13 +2682,13 @@
         <v>152</v>
       </c>
       <c r="B122" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C122" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="D122" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.2">
@@ -2660,13 +2696,13 @@
         <v>152</v>
       </c>
       <c r="B123" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C123" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D123" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.2">
@@ -2674,13 +2710,13 @@
         <v>152</v>
       </c>
       <c r="B124" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C124" t="s">
-        <v>84</v>
+        <v>0</v>
       </c>
       <c r="D124" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.2">
@@ -2688,13 +2724,13 @@
         <v>152</v>
       </c>
       <c r="B125" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C125" t="s">
-        <v>0</v>
+        <v>93</v>
       </c>
       <c r="D125" t="s">
-        <v>87</v>
+        <v>186</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.2">
@@ -2702,13 +2738,10 @@
         <v>152</v>
       </c>
       <c r="B126" t="s">
-        <v>86</v>
-      </c>
-      <c r="C126" t="s">
-        <v>93</v>
+        <v>115</v>
       </c>
       <c r="D126" t="s">
-        <v>94</v>
+        <v>160</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.2">
@@ -2716,10 +2749,13 @@
         <v>152</v>
       </c>
       <c r="B127" t="s">
-        <v>78</v>
+        <v>115</v>
+      </c>
+      <c r="C127" t="s">
+        <v>0</v>
       </c>
       <c r="D127" t="s">
-        <v>167</v>
+        <v>128</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.2">
@@ -2727,13 +2763,13 @@
         <v>152</v>
       </c>
       <c r="B128" t="s">
-        <v>78</v>
+        <v>115</v>
       </c>
       <c r="C128" t="s">
-        <v>0</v>
+        <v>116</v>
       </c>
       <c r="D128" t="s">
-        <v>79</v>
+        <v>130</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.2">
@@ -2741,13 +2777,10 @@
         <v>152</v>
       </c>
       <c r="B129" t="s">
-        <v>78</v>
-      </c>
-      <c r="C129" t="s">
-        <v>20</v>
+        <v>86</v>
       </c>
       <c r="D129" t="s">
-        <v>80</v>
+        <v>164</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.2">
@@ -2755,10 +2788,13 @@
         <v>152</v>
       </c>
       <c r="B130" t="s">
-        <v>117</v>
+        <v>86</v>
+      </c>
+      <c r="C130" t="s">
+        <v>88</v>
       </c>
       <c r="D130" t="s">
-        <v>169</v>
+        <v>89</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.2">
@@ -2766,13 +2802,13 @@
         <v>152</v>
       </c>
       <c r="B131" t="s">
-        <v>117</v>
+        <v>86</v>
       </c>
       <c r="C131" t="s">
         <v>83</v>
       </c>
       <c r="D131" t="s">
-        <v>119</v>
+        <v>90</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.2">
@@ -2780,13 +2816,13 @@
         <v>152</v>
       </c>
       <c r="B132" t="s">
-        <v>117</v>
+        <v>86</v>
       </c>
       <c r="C132" t="s">
         <v>84</v>
       </c>
       <c r="D132" t="s">
-        <v>120</v>
+        <v>91</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.2">
@@ -2794,13 +2830,13 @@
         <v>152</v>
       </c>
       <c r="B133" t="s">
-        <v>117</v>
+        <v>86</v>
       </c>
       <c r="C133" t="s">
         <v>0</v>
       </c>
       <c r="D133" t="s">
-        <v>118</v>
+        <v>87</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.2">
@@ -2808,12 +2844,118 @@
         <v>152</v>
       </c>
       <c r="B134" t="s">
-        <v>117</v>
+        <v>86</v>
       </c>
       <c r="C134" t="s">
         <v>93</v>
       </c>
       <c r="D134" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A135" t="s">
+        <v>152</v>
+      </c>
+      <c r="B135" t="s">
+        <v>78</v>
+      </c>
+      <c r="D135" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A136" t="s">
+        <v>152</v>
+      </c>
+      <c r="B136" t="s">
+        <v>78</v>
+      </c>
+      <c r="C136" t="s">
+        <v>0</v>
+      </c>
+      <c r="D136" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A137" t="s">
+        <v>152</v>
+      </c>
+      <c r="B137" t="s">
+        <v>78</v>
+      </c>
+      <c r="C137" t="s">
+        <v>20</v>
+      </c>
+      <c r="D137" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A138" t="s">
+        <v>152</v>
+      </c>
+      <c r="B138" t="s">
+        <v>117</v>
+      </c>
+      <c r="D138" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A139" t="s">
+        <v>152</v>
+      </c>
+      <c r="B139" t="s">
+        <v>117</v>
+      </c>
+      <c r="C139" t="s">
+        <v>83</v>
+      </c>
+      <c r="D139" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A140" t="s">
+        <v>152</v>
+      </c>
+      <c r="B140" t="s">
+        <v>117</v>
+      </c>
+      <c r="C140" t="s">
+        <v>84</v>
+      </c>
+      <c r="D140" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A141" t="s">
+        <v>152</v>
+      </c>
+      <c r="B141" t="s">
+        <v>117</v>
+      </c>
+      <c r="C141" t="s">
+        <v>0</v>
+      </c>
+      <c r="D141" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A142" t="s">
+        <v>152</v>
+      </c>
+      <c r="B142" t="s">
+        <v>117</v>
+      </c>
+      <c r="C142" t="s">
+        <v>93</v>
+      </c>
+      <c r="D142" t="s">
         <v>121</v>
       </c>
     </row>

</xml_diff>